<commit_message>
pryecto terminado para presentacion
</commit_message>
<xml_diff>
--- a/SisRestaurant/src/main/resources/doc/plantilla_importacio.xlsx
+++ b/SisRestaurant/src/main/resources/doc/plantilla_importacio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\ProyectoPrueva\SisRestaurant\src\main\resources\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC9DBA6-BEB5-4E11-8040-D349123FFB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4F9FF0-BD7B-45CD-918B-FD7570FE07FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>--- CATEGORIAS ---</t>
   </si>
@@ -55,19 +55,25 @@
     <t>--- TIPO DOC VENTA ---</t>
   </si>
   <si>
-    <t>plato</t>
+    <t>Ciglas</t>
+  </si>
+  <si>
+    <t>platos</t>
   </si>
   <si>
     <t>lunes</t>
   </si>
   <si>
-    <t>dni</t>
+    <t>DNI</t>
   </si>
   <si>
     <t>administrador</t>
   </si>
   <si>
-    <t>boleta</t>
+    <t>Boleta</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>sopa</t>
@@ -76,40 +82,40 @@
     <t>martes</t>
   </si>
   <si>
-    <t>ruc</t>
+    <t>RUC</t>
   </si>
   <si>
     <t>cajero</t>
   </si>
   <si>
-    <t>factura</t>
+    <t>Factura</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>entrada</t>
+  </si>
+  <si>
+    <t>jueves</t>
+  </si>
+  <si>
+    <t>carnet extrajero</t>
+  </si>
+  <si>
+    <t>contador</t>
+  </si>
+  <si>
+    <t>nota de Venta</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>postre</t>
   </si>
   <si>
     <t>bebidas</t>
-  </si>
-  <si>
-    <t>jueves</t>
-  </si>
-  <si>
-    <t>pasaport</t>
-  </si>
-  <si>
-    <t>contador</t>
-  </si>
-  <si>
-    <t>nota de venta</t>
-  </si>
-  <si>
-    <t>Ciglas</t>
-  </si>
-  <si>
-    <t>B001</t>
-  </si>
-  <si>
-    <t>F001</t>
-  </si>
-  <si>
-    <t>N001</t>
   </si>
 </sst>
 </file>
@@ -483,9 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -497,6 +501,7 @@
     <col min="9" max="9" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -545,12 +550,12 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -559,27 +564,27 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I3">
         <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -588,27 +593,27 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -617,25 +622,28 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="N5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
       <c r="C6">
         <v>4</v>
       </c>
@@ -644,6 +652,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
       <c r="C7">
         <v>5</v>
       </c>

</xml_diff>